<commit_message>
updated BOM with proper connector
</commit_message>
<xml_diff>
--- a/pcb/R1008_BOM.xlsx
+++ b/pcb/R1008_BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
   <si>
     <t>Reference</t>
   </si>
@@ -95,7 +95,10 @@
     <t>Main:70553-0038</t>
   </si>
   <si>
-    <t>Phoenix Contact</t>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>70553-0038</t>
   </si>
   <si>
     <t>J4 J6 </t>
@@ -284,15 +287,15 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.37755102040816"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.2959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.1785714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.1989795918367"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.76530612244898"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6071428571429"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.6581632653061"/>
@@ -401,8 +404,8 @@
       <c r="F3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="0" t="n">
-        <v>1725672</v>
+      <c r="G3" s="0" t="s">
+        <v>27</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>18</v>
@@ -410,22 +413,22 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>18</v>
@@ -433,118 +436,118 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>17</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D6" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="H6" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>17</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D8" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>49</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>18</v>
@@ -552,22 +555,22 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>18</v>
@@ -575,11 +578,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>